<commit_message>
revision, added pyrolysis and additional figures
</commit_message>
<xml_diff>
--- a/data/raw/master_file_health_large_biomass.xlsx
+++ b/data/raw/master_file_health_large_biomass.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huo\Documents\GitHub\polyLOP\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C130F4-A4B4-44FE-ACD9-6FEB0460DDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10965" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="product" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="process_ihs" sheetId="6" r:id="rId8"/>
     <sheet name="flows_o" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
@@ -30,17 +31,28 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jing Huo</author>
   </authors>
   <commentList>
-    <comment ref="F10" authorId="0" shapeId="0">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F53" authorId="0" shapeId="0">
+    <comment ref="F53" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F64" authorId="0" shapeId="0">
+    <comment ref="F64" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F73" authorId="0" shapeId="0">
+    <comment ref="F73" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F110" authorId="0" shapeId="0">
+    <comment ref="F110" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -216,12 +228,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jing Huo</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -250,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11024" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11016" uniqueCount="767">
   <si>
     <t>electricity</t>
   </si>
@@ -2581,9 +2593,6 @@
     <t>methanol, from agricultural residue gasification, with co2 capture, according to Charalambous</t>
   </si>
   <si>
-    <t>heat</t>
-  </si>
-  <si>
     <t>nox_emission_energy</t>
   </si>
   <si>
@@ -2647,7 +2656,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3094,7 +3103,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jing Huo" refreshedDate="45365.652996990742" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="626">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jing Huo" refreshedDate="45365.652996990742" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="626" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -8968,7 +8977,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0900-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:E619" firstHeaderRow="1" firstDataRow="1" firstDataCol="4"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -12424,117 +12433,136 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F118" totalsRowShown="0">
-  <autoFilter ref="A1:F118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:F118" totalsRowShown="0">
+  <autoFilter ref="A1:F118" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="emission"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:F110">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F110">
     <sortCondition ref="A1:A110"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="product_name" dataDxfId="23"/>
-    <tableColumn id="2" name="unit"/>
-    <tableColumn id="5" name="product_type"/>
-    <tableColumn id="3" name="include"/>
-    <tableColumn id="4" name="raw_material_type"/>
-    <tableColumn id="6" name="carbon_content"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="product_name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="unit"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="product_type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="include"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="raw_material_type"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="carbon_content"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N109" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:N109"/>
-  <sortState ref="A2:N103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:N109" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A1:N109" xr:uid="{00000000-0009-0000-0100-000003000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="methanol, from agricultural residue gasification, base"/>
+        <filter val="methanol, from agricultural residue gasification, beccs"/>
+        <filter val="methanol, from agricultural residue gasification, combined with co2 hydrogenation"/>
+        <filter val="methanol, from agricultural residue gasification, with co2 capture"/>
+        <filter val="methanol, from agricultural residue gasification, with co2 capture, according to Charalambous"/>
+        <filter val="methanol, from agricultural residue gasification, without co2 capture"/>
+        <filter val="methanol, from co2 hydrogenation"/>
+        <filter val="methanol, from forest residue gasification, base"/>
+        <filter val="methanol, from forest residue gasification, beccs"/>
+        <filter val="methanol, from forest residue gasification, combined with co2 hydrogenation"/>
+        <filter val="methanol, from forest residue gasification, with co2 capture"/>
+        <filter val="methanol, from forest residue gasification, with co2 capture, according to Charalambous"/>
+        <filter val="methanol, from forest residue gasification, without co2 capture"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N103">
     <sortCondition ref="A1:A103"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="product_process" dataDxfId="21"/>
-    <tableColumn id="2" name="product_name" dataDxfId="20"/>
-    <tableColumn id="5" name="process" dataDxfId="19"/>
-    <tableColumn id="6" name="ratio" dataDxfId="18"/>
-    <tableColumn id="3" name="TRL" dataDxfId="17"/>
-    <tableColumn id="4" name="Data source" dataDxfId="16"/>
-    <tableColumn id="7" name="include" dataDxfId="15"/>
-    <tableColumn id="8" name="note" dataDxfId="14"/>
-    <tableColumn id="9" name="co2_route" dataDxfId="13"/>
-    <tableColumn id="10" name="agricultural_residue_route" dataDxfId="12"/>
-    <tableColumn id="12" name="forest_residue_route" dataDxfId="11"/>
-    <tableColumn id="11" name="fossil_route" dataDxfId="10"/>
-    <tableColumn id="14" name="chemical_recycling_route" dataDxfId="9"/>
-    <tableColumn id="13" name="all" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="product_process" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="product_name" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="process" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="ratio" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TRL" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Data source" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="include" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="note" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="co2_route" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="agricultural_residue_route" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="forest_residue_route" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="fossil_route" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="chemical_recycling_route" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="all" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E680" totalsRowShown="0">
-  <autoFilter ref="A1:E680">
-    <filterColumn colId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table6" displayName="Table6" ref="A1:E678" totalsRowShown="0">
+  <autoFilter ref="A1:E678" xr:uid="{00000000-0009-0000-0100-000006000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="nox_emission_energy"/>
-        <filter val="pm25_emission_energy"/>
-        <filter val="refrigerant_energy"/>
-        <filter val="sox_emission_energy"/>
+        <filter val="methanol, from agricultural residue gasification, with co2 capture, according to Charalambous"/>
+        <filter val="methanol, from forest residue gasification, with co2 capture, according to Charalambous"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A115:E659">
-    <sortCondition ref="A1:A676"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A115:E659">
+    <sortCondition ref="A1:A674"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="process"/>
-    <tableColumn id="2" name="product_name"/>
-    <tableColumn id="3" name="type"/>
-    <tableColumn id="4" name="unit"/>
-    <tableColumn id="5" name="value"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="process"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="product_name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="unit"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J105" totalsRowShown="0">
-  <autoFilter ref="A1:J105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A1:J105" totalsRowShown="0">
+  <autoFilter ref="A1:J105" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="9">
       <filters>
         <filter val="yes"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:J107">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J107">
     <sortCondition ref="D1:D107"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="product_name"/>
-    <tableColumn id="2" name="technology"/>
-    <tableColumn id="3" name="pollutant"/>
-    <tableColumn id="4" name="unit"/>
-    <tableColumn id="5" name="value"/>
-    <tableColumn id="6" name="value_lower"/>
-    <tableColumn id="7" name="value_upper"/>
-    <tableColumn id="8" name="source"/>
-    <tableColumn id="9" name="link"/>
-    <tableColumn id="10" name="include"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="product_name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="technology"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="pollutant"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="unit"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="value"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="value_lower"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="value_upper"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="source"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="link"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="include"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:U100" totalsRowShown="0">
-  <autoFilter ref="A1:U100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table4" displayName="Table4" ref="A1:U100" totalsRowShown="0">
+  <autoFilter ref="A1:U100" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="no"/>
@@ -12546,50 +12574,50 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:T100">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T100">
     <sortCondition ref="A1:A100"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="product"/>
-    <tableColumn id="2" name="process"/>
-    <tableColumn id="3" name="dominant"/>
-    <tableColumn id="4" name="include"/>
-    <tableColumn id="20" name="include_o"/>
-    <tableColumn id="13" name="Comment CO"/>
-    <tableColumn id="14" name="Column1"/>
-    <tableColumn id="5" name="number_of_data"/>
-    <tableColumn id="6" name="note_process"/>
-    <tableColumn id="7" name="reference"/>
-    <tableColumn id="8" name="co-products"/>
-    <tableColumn id="9" name="note_coproduction"/>
-    <tableColumn id="10" name="process_ghg_emission"/>
-    <tableColumn id="11" name="process_ghg_emission_amount"/>
-    <tableColumn id="12" name="process_ghg_emission_reference"/>
-    <tableColumn id="15" name="co2_route"/>
-    <tableColumn id="16" name="agricultural_residue_route"/>
-    <tableColumn id="17" name="forest_residue_route"/>
-    <tableColumn id="18" name="fossil_route"/>
-    <tableColumn id="21" name="chemical_recycling_route"/>
-    <tableColumn id="19" name="all"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="product"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="process"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="dominant"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="include"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="include_o"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Comment CO"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="Column1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="number_of_data"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="note_process"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="reference"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="co-products"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="note_coproduction"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="process_ghg_emission"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="process_ghg_emission_amount"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="process_ghg_emission_reference"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="co2_route"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="agricultural_residue_route"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="forest_residue_route"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="fossil_route"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="chemical_recycling_route"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="all"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G627" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G627"/>
-  <sortState ref="A2:F196">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table1" displayName="Table1" ref="A1:G627" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G627" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F196">
     <sortCondition ref="A1:A196"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="process" dataDxfId="6"/>
-    <tableColumn id="8" name="type" dataDxfId="5"/>
-    <tableColumn id="2" name="product_name" dataDxfId="4"/>
-    <tableColumn id="3" name="value" dataDxfId="3"/>
-    <tableColumn id="4" name="unit" dataDxfId="2"/>
-    <tableColumn id="5" name="checked" dataDxfId="1"/>
-    <tableColumn id="6" name="note" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="process" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="type" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="product_name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="value" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="unit" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="checked" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12857,7 +12885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14885,7 +14913,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B111" t="s">
         <v>14</v>
@@ -14902,7 +14930,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="38" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B112" t="s">
         <v>14</v>
@@ -14919,7 +14947,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="38" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B113" t="s">
         <v>14</v>
@@ -14936,7 +14964,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="38" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B114" t="s">
         <v>14</v>
@@ -14953,7 +14981,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="38" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B115" t="s">
         <v>14</v>
@@ -14970,7 +14998,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="38" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B116" t="s">
         <v>14</v>
@@ -14987,7 +15015,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="38" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B117" t="s">
         <v>14</v>
@@ -15004,7 +15032,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="38" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B118" t="s">
         <v>14</v>
@@ -15030,11 +15058,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15088,7 +15116,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>607</v>
       </c>
@@ -15118,7 +15146,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -15146,7 +15174,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -15174,7 +15202,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -15202,7 +15230,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -15230,7 +15258,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -15258,7 +15286,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -15286,7 +15314,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -15314,7 +15342,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -15342,7 +15370,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
@@ -15370,7 +15398,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>139</v>
       </c>
@@ -15398,7 +15426,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>67</v>
       </c>
@@ -15436,7 +15464,7 @@
       </c>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>605</v>
       </c>
@@ -15466,7 +15494,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>614</v>
       </c>
@@ -15496,7 +15524,7 @@
       </c>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>506</v>
       </c>
@@ -15526,7 +15554,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>199</v>
       </c>
@@ -15556,7 +15584,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>511</v>
       </c>
@@ -15584,7 +15612,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>513</v>
       </c>
@@ -15612,7 +15640,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>514</v>
       </c>
@@ -15640,7 +15668,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>515</v>
       </c>
@@ -15668,7 +15696,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
@@ -15696,7 +15724,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>120</v>
       </c>
@@ -15724,7 +15752,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>722</v>
       </c>
@@ -15752,7 +15780,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>721</v>
       </c>
@@ -15780,7 +15808,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>710</v>
       </c>
@@ -15808,7 +15836,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>708</v>
       </c>
@@ -15836,7 +15864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>707</v>
       </c>
@@ -15864,7 +15892,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>178</v>
       </c>
@@ -15892,7 +15920,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>122</v>
       </c>
@@ -15920,7 +15948,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>123</v>
       </c>
@@ -15948,7 +15976,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>606</v>
       </c>
@@ -15978,7 +16006,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>156</v>
       </c>
@@ -16010,7 +16038,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>128</v>
       </c>
@@ -16038,7 +16066,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>157</v>
       </c>
@@ -16070,7 +16098,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>129</v>
       </c>
@@ -16098,7 +16126,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>126</v>
       </c>
@@ -16126,7 +16154,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>127</v>
       </c>
@@ -16154,7 +16182,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>124</v>
       </c>
@@ -16182,7 +16210,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>125</v>
       </c>
@@ -16210,7 +16238,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>130</v>
       </c>
@@ -16238,7 +16266,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>131</v>
       </c>
@@ -16266,7 +16294,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>171</v>
       </c>
@@ -16296,7 +16324,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -16334,7 +16362,7 @@
       </c>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>726</v>
       </c>
@@ -16364,7 +16392,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>135</v>
       </c>
@@ -16396,7 +16424,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>136</v>
       </c>
@@ -16428,7 +16456,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>133</v>
       </c>
@@ -16460,7 +16488,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>161</v>
       </c>
@@ -16492,7 +16520,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>134</v>
       </c>
@@ -16524,7 +16552,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>164</v>
       </c>
@@ -16556,7 +16584,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>26</v>
       </c>
@@ -16584,7 +16612,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>28</v>
       </c>
@@ -16612,7 +16640,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>27</v>
       </c>
@@ -16638,7 +16666,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>24</v>
       </c>
@@ -16662,7 +16690,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>29</v>
       </c>
@@ -16688,7 +16716,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>95</v>
       </c>
@@ -16716,7 +16744,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>96</v>
       </c>
@@ -16744,7 +16772,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>35</v>
       </c>
@@ -16772,7 +16800,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>109</v>
       </c>
@@ -16800,7 +16828,7 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>111</v>
       </c>
@@ -17016,7 +17044,7 @@
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>594</v>
       </c>
@@ -17044,7 +17072,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>87</v>
       </c>
@@ -17072,7 +17100,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>90</v>
       </c>
@@ -17100,7 +17128,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
@@ -17132,7 +17160,7 @@
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>162</v>
       </c>
@@ -17164,7 +17192,7 @@
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>138</v>
       </c>
@@ -17196,7 +17224,7 @@
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>165</v>
       </c>
@@ -17228,7 +17256,7 @@
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>140</v>
       </c>
@@ -17256,7 +17284,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>141</v>
       </c>
@@ -17284,7 +17312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>727</v>
       </c>
@@ -17314,7 +17342,7 @@
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>728</v>
       </c>
@@ -17344,7 +17372,7 @@
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>729</v>
       </c>
@@ -17374,7 +17402,7 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>179</v>
       </c>
@@ -17402,7 +17430,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>45</v>
       </c>
@@ -17440,7 +17468,7 @@
       </c>
       <c r="N82" s="2"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>75</v>
       </c>
@@ -17478,7 +17506,7 @@
       </c>
       <c r="N83" s="2"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>210</v>
       </c>
@@ -17514,7 +17542,7 @@
       </c>
       <c r="N84" s="2"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>50</v>
       </c>
@@ -17542,7 +17570,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>49</v>
       </c>
@@ -17570,7 +17598,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>609</v>
       </c>
@@ -17600,7 +17628,7 @@
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>105</v>
       </c>
@@ -17628,7 +17656,7 @@
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>108</v>
       </c>
@@ -17656,7 +17684,7 @@
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>114</v>
       </c>
@@ -17684,7 +17712,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>203</v>
       </c>
@@ -17712,7 +17740,7 @@
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>206</v>
       </c>
@@ -17740,7 +17768,7 @@
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>504</v>
       </c>
@@ -17776,7 +17804,7 @@
       </c>
       <c r="N93" s="2"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>474</v>
       </c>
@@ -17812,7 +17840,7 @@
       </c>
       <c r="N94" s="2"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>615</v>
       </c>
@@ -17842,7 +17870,7 @@
       </c>
       <c r="N95" s="2"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>473</v>
       </c>
@@ -17878,7 +17906,7 @@
       </c>
       <c r="N96" s="2"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>237</v>
       </c>
@@ -17908,7 +17936,7 @@
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>72</v>
       </c>
@@ -17946,7 +17974,7 @@
       </c>
       <c r="N98" s="2"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>103</v>
       </c>
@@ -17978,7 +18006,7 @@
       </c>
       <c r="N99" s="2"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>159</v>
       </c>
@@ -18011,7 +18039,7 @@
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>160</v>
       </c>
@@ -18044,7 +18072,7 @@
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>142</v>
       </c>
@@ -18076,7 +18104,7 @@
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>143</v>
       </c>
@@ -18232,7 +18260,7 @@
       <c r="E108" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F108" s="9" t="s">
         <v>744</v>
       </c>
       <c r="G108" s="2" t="s">
@@ -18278,23 +18306,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F49" r:id="rId1"/>
-    <hyperlink ref="F45" r:id="rId2" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="F44" r:id="rId3"/>
-    <hyperlink ref="F79" r:id="rId4"/>
-    <hyperlink ref="F52" r:id="rId5"/>
-    <hyperlink ref="F35" r:id="rId6"/>
+    <hyperlink ref="F49" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F45" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F44" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F79" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="F52" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="F35" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="F108" r:id="rId7" xr:uid="{46323171-7C3A-4B4D-ABDD-53DC6EB1684F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:E619"/>
   <sheetViews>
     <sheetView topLeftCell="A586" workbookViewId="0">
@@ -28805,11 +28834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U680"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:U678"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E629" sqref="E629"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B685" sqref="B685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33326,7 +33355,7 @@
         <v>-1.6779120000000001</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>171</v>
       </c>
@@ -35302,12 +35331,12 @@
       </c>
       <c r="H379" s="33"/>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>708</v>
       </c>
       <c r="B380" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C380" t="s">
         <v>500</v>
@@ -36707,12 +36736,12 @@
       </c>
       <c r="H457" s="33"/>
     </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>708</v>
       </c>
       <c r="B458" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C458" t="s">
         <v>500</v>
@@ -37050,12 +37079,12 @@
       </c>
       <c r="H476" s="33"/>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>708</v>
       </c>
       <c r="B477" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C477" t="s">
         <v>500</v>
@@ -38365,12 +38394,12 @@
       </c>
       <c r="H549" s="33"/>
     </row>
-    <row r="550" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>707</v>
       </c>
       <c r="B550" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C550" t="s">
         <v>500</v>
@@ -38600,12 +38629,12 @@
       </c>
       <c r="H562" s="33"/>
     </row>
-    <row r="563" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>707</v>
       </c>
       <c r="B563" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C563" t="s">
         <v>500</v>
@@ -38709,12 +38738,12 @@
       </c>
       <c r="H568" s="33"/>
     </row>
-    <row r="569" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>707</v>
       </c>
       <c r="B569" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C569" t="s">
         <v>500</v>
@@ -39664,12 +39693,12 @@
       </c>
       <c r="H621" s="33"/>
     </row>
-    <row r="622" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>26</v>
       </c>
       <c r="B622" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C622" t="s">
         <v>500</v>
@@ -39683,12 +39712,12 @@
       </c>
       <c r="H622" s="33"/>
     </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>26</v>
       </c>
       <c r="B623" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C623" t="s">
         <v>500</v>
@@ -39702,12 +39731,12 @@
       </c>
       <c r="H623" s="33"/>
     </row>
-    <row r="624" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>26</v>
       </c>
       <c r="B624" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C624" t="s">
         <v>500</v>
@@ -39757,12 +39786,12 @@
       </c>
       <c r="H626" s="33"/>
     </row>
-    <row r="627" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>28</v>
       </c>
       <c r="B627" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C627" t="s">
         <v>500</v>
@@ -39776,12 +39805,12 @@
       </c>
       <c r="H627" s="33"/>
     </row>
-    <row r="628" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
         <v>28</v>
       </c>
       <c r="B628" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C628" t="s">
         <v>500</v>
@@ -39795,12 +39824,12 @@
       </c>
       <c r="H628" s="33"/>
     </row>
-    <row r="629" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
         <v>28</v>
       </c>
       <c r="B629" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C629" t="s">
         <v>500</v>
@@ -40296,7 +40325,7 @@
         <v>594</v>
       </c>
       <c r="B658" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C658" t="s">
         <v>500</v>
@@ -40313,7 +40342,7 @@
         <v>114</v>
       </c>
       <c r="B659" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C659" t="s">
         <v>500</v>
@@ -40342,7 +40371,7 @@
         <v>1.7777999999999999E-2</v>
       </c>
     </row>
-    <row r="661" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A661" s="2" t="s">
         <v>745</v>
       </c>
@@ -40359,7 +40388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="662" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A662" s="2" t="s">
         <v>745</v>
       </c>
@@ -40376,63 +40405,63 @@
         <v>-0.15488000000000002</v>
       </c>
     </row>
-    <row r="663" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A663" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="B663" s="6" t="s">
-        <v>747</v>
+      <c r="B663" t="s">
+        <v>1</v>
       </c>
       <c r="C663" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D663" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E663">
-        <v>-7.1999999999999993</v>
-      </c>
-    </row>
-    <row r="664" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.9901457882413798</v>
+      </c>
+    </row>
+    <row r="664" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A664" s="2" t="s">
         <v>745</v>
       </c>
       <c r="B664" t="s">
-        <v>1</v>
+        <v>613</v>
       </c>
       <c r="C664" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D664" t="s">
         <v>14</v>
       </c>
       <c r="E664">
-        <v>-1.9901457882413798</v>
-      </c>
-    </row>
-    <row r="665" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="665" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A665" s="2" t="s">
         <v>745</v>
       </c>
       <c r="B665" t="s">
-        <v>613</v>
+        <v>30</v>
       </c>
       <c r="C665" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D665" t="s">
         <v>14</v>
       </c>
       <c r="E665">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="666" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="666" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A666" s="2" t="s">
         <v>745</v>
       </c>
       <c r="B666" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C666" t="s">
         <v>500</v>
@@ -40441,151 +40470,151 @@
         <v>14</v>
       </c>
       <c r="E666">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="667" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.0668418374704494</v>
+      </c>
+    </row>
+    <row r="667" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A667" s="2" t="s">
         <v>745</v>
       </c>
       <c r="B667" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C667" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D667" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E667">
-        <v>1.0668418374704494</v>
-      </c>
-    </row>
-    <row r="668" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>-4.3520000000000003</v>
+      </c>
+    </row>
+    <row r="668" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A668" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B668" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C668" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D668" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E668">
-        <v>-4.3520000000000003</v>
-      </c>
-    </row>
-    <row r="669" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="669" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A669" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B669" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C669" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D669" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E669">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="670" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.15488000000000002</v>
+      </c>
+    </row>
+    <row r="670" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A670" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B670" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C670" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D670" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E670">
-        <v>-0.15488000000000002</v>
-      </c>
-    </row>
-    <row r="671" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.9901457882413798</v>
+      </c>
+    </row>
+    <row r="671" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A671" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B671" t="s">
-        <v>747</v>
+        <v>613</v>
       </c>
       <c r="C671" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="D671" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E671">
-        <v>-7.1999999999999993</v>
-      </c>
-    </row>
-    <row r="672" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="672" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A672" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B672" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C672" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D672" t="s">
         <v>14</v>
       </c>
       <c r="E672">
-        <v>-1.9901457882413798</v>
-      </c>
-    </row>
-    <row r="673" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="673" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A673" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B673" t="s">
-        <v>613</v>
+        <v>31</v>
       </c>
       <c r="C673" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D673" t="s">
         <v>14</v>
       </c>
       <c r="E673">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="674" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.86981740443455269</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A674" s="2" t="s">
         <v>746</v>
       </c>
       <c r="B674" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C674" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D674" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E674">
-        <v>0.13</v>
+        <v>-4.3520000000000003</v>
       </c>
     </row>
     <row r="675" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A675" s="2" t="s">
-        <v>746</v>
+      <c r="A675" t="s">
+        <v>28</v>
       </c>
       <c r="B675" t="s">
-        <v>31</v>
+        <v>752</v>
       </c>
       <c r="C675" t="s">
         <v>500</v>
@@ -40594,32 +40623,32 @@
         <v>14</v>
       </c>
       <c r="E675">
-        <v>0.86981740443455269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="676" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A676" s="2" t="s">
-        <v>746</v>
+      <c r="A676" t="s">
+        <v>26</v>
       </c>
       <c r="B676" t="s">
-        <v>65</v>
+        <v>752</v>
       </c>
       <c r="C676" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D676" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E676">
-        <v>-4.3520000000000003</v>
-      </c>
-    </row>
-    <row r="677" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>28</v>
+        <v>708</v>
       </c>
       <c r="B677" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C677" t="s">
         <v>500</v>
@@ -40631,12 +40660,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="678" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>26</v>
+        <v>707</v>
       </c>
       <c r="B678" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C678" t="s">
         <v>500</v>
@@ -40645,40 +40674,6 @@
         <v>14</v>
       </c>
       <c r="E678">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="679" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A679" t="s">
-        <v>708</v>
-      </c>
-      <c r="B679" t="s">
-        <v>753</v>
-      </c>
-      <c r="C679" t="s">
-        <v>500</v>
-      </c>
-      <c r="D679" t="s">
-        <v>14</v>
-      </c>
-      <c r="E679">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="680" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A680" t="s">
-        <v>707</v>
-      </c>
-      <c r="B680" t="s">
-        <v>753</v>
-      </c>
-      <c r="C680" t="s">
-        <v>500</v>
-      </c>
-      <c r="D680" t="s">
-        <v>14</v>
-      </c>
-      <c r="E680">
         <v>0</v>
       </c>
     </row>
@@ -40691,10 +40686,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -40717,13 +40712,13 @@
         <v>0</v>
       </c>
       <c r="J1" t="s">
+        <v>761</v>
+      </c>
+      <c r="K1" t="s">
         <v>762</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>763</v>
-      </c>
-      <c r="L1" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -40735,10 +40730,10 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
+        <v>757</v>
+      </c>
+      <c r="I2" t="s">
         <v>758</v>
-      </c>
-      <c r="I2" t="s">
-        <v>759</v>
       </c>
       <c r="J2">
         <v>57</v>
@@ -40750,7 +40745,7 @@
         <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="N2" s="33">
         <v>9.9999999999999995E-7</v>
@@ -40761,7 +40756,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C3" s="33">
         <f>$C$2*J2*$N$2</f>
@@ -40772,7 +40767,7 @@
         <v>7.1999999999999994E-4</v>
       </c>
       <c r="I3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J3">
         <v>57</v>
@@ -40786,10 +40781,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C4" s="33">
-        <f t="shared" ref="C4:D6" si="0">$C$2*J3*$N$2</f>
+        <f t="shared" ref="C4:D5" si="0">$C$2*J3*$N$2</f>
         <v>5.4000000000000001E-4</v>
       </c>
       <c r="D4" s="33">
@@ -40797,7 +40792,7 @@
         <v>2.330526315789473E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="J4">
         <v>8</v>
@@ -40811,7 +40806,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C5" s="33">
         <f t="shared" si="0"/>
@@ -40825,18 +40820,18 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="33"/>
       <c r="L6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="N6">
         <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="L7" s="33">
         <f>L2*$N$2*$N$6</f>
@@ -40854,10 +40849,10 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L8" s="33">
         <f t="shared" ref="L8:L9" si="1">L3*$N$2*$N$6</f>
@@ -40876,10 +40871,10 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I9" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="L9" s="33">
         <f t="shared" si="1"/>
@@ -40891,7 +40886,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C10" s="33">
         <f>$C$9*J2*$N$2</f>
@@ -40904,7 +40899,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C11" s="33">
         <f t="shared" ref="C11:D11" si="2">$C$9*J3*$N$2</f>
@@ -40917,7 +40912,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C12" s="33">
         <f t="shared" ref="C12:D12" si="3">$C$9*J4*$N$2</f>
@@ -40934,7 +40929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
@@ -44263,13 +44258,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I99" r:id="rId1"/>
-    <hyperlink ref="I103" r:id="rId2"/>
-    <hyperlink ref="I18" r:id="rId3"/>
-    <hyperlink ref="I42" r:id="rId4"/>
-    <hyperlink ref="I54" r:id="rId5"/>
-    <hyperlink ref="I19" r:id="rId6"/>
-    <hyperlink ref="I90" r:id="rId7"/>
+    <hyperlink ref="I99" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="I103" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="I18" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="I42" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="I54" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="I19" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="I90" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -44279,7 +44274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -44490,7 +44485,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -44499,7 +44494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -48775,14 +48770,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J31" r:id="rId2"/>
-    <hyperlink ref="J29" r:id="rId3"/>
-    <hyperlink ref="J41" r:id="rId4"/>
-    <hyperlink ref="J87" r:id="rId5"/>
-    <hyperlink ref="J5" r:id="rId6"/>
-    <hyperlink ref="J36" r:id="rId7"/>
-    <hyperlink ref="J39" r:id="rId8"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="J31" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="J29" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="J41" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="J87" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="J36" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="J39" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -48793,7 +48788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G627"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">

</xml_diff>